<commit_message>
oppdaterer printReslts. Klargjør for testing.
</commit_message>
<xml_diff>
--- a/clusterCurrentSolution.xlsx
+++ b/clusterCurrentSolution.xlsx
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B202"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C159"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -360,9 +360,17 @@
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -370,7 +378,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -378,7 +386,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -386,7 +394,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -394,7 +402,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -402,7 +410,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -410,7 +418,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -418,7 +426,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -426,7 +434,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -434,7 +442,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -442,7 +450,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -450,7 +458,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -458,7 +466,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -466,7 +474,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -474,7 +482,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -482,7 +490,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -490,7 +498,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -498,7 +506,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -506,7 +514,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -514,7 +522,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -522,7 +530,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -530,7 +538,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -538,7 +546,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -546,7 +554,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -554,7 +562,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -562,7 +570,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -570,7 +578,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -578,7 +586,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -586,7 +594,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -594,7 +602,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -602,7 +610,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -610,7 +618,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -618,7 +626,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -626,7 +634,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -634,7 +642,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -642,7 +650,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -650,7 +658,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -658,7 +666,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -666,7 +674,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -674,7 +682,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -682,7 +690,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -690,7 +698,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -698,7 +706,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -706,7 +714,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -714,7 +722,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -722,7 +730,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -730,7 +738,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -738,7 +746,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -746,7 +754,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -754,7 +762,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -762,7 +770,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -770,7 +778,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -778,7 +786,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -786,7 +794,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -794,7 +802,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -802,7 +810,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -810,7 +818,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -818,7 +826,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -826,7 +834,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -834,7 +842,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -842,7 +850,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -850,7 +858,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -858,7 +866,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -866,7 +874,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -874,7 +882,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -882,7 +890,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -890,7 +898,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -898,7 +906,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -906,7 +914,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -914,7 +922,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -922,7 +930,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -930,7 +938,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -938,7 +946,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -946,7 +954,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -954,7 +962,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -962,7 +970,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -970,7 +978,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -978,7 +986,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -986,7 +994,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -994,7 +1002,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1002,7 +1010,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1010,7 +1018,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1018,7 +1026,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1026,7 +1034,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1034,7 +1042,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1042,7 +1050,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1050,7 +1058,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1058,7 +1066,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1066,7 +1074,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1074,7 +1082,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1082,7 +1090,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1090,7 +1098,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1098,7 +1106,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1106,7 +1114,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1114,7 +1122,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1122,7 +1130,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -1130,7 +1138,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -1138,7 +1146,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -1146,7 +1154,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -1154,7 +1162,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -1162,7 +1170,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -1170,7 +1178,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -1178,7 +1186,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -1186,7 +1194,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -1194,7 +1202,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1202,7 +1210,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -1210,7 +1218,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -1218,7 +1226,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -1226,7 +1234,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -1234,7 +1242,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -1242,7 +1250,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -1250,7 +1258,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -1258,7 +1266,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -1266,7 +1274,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -1274,7 +1282,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -1282,7 +1290,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -1290,7 +1298,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -1298,7 +1306,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -1306,7 +1314,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -1314,7 +1322,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -1322,7 +1330,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -1330,7 +1338,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -1338,7 +1346,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -1346,7 +1354,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -1354,7 +1362,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -1362,7 +1370,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -1370,7 +1378,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -1378,7 +1386,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -1386,7 +1394,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -1394,7 +1402,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -1402,7 +1410,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -1410,7 +1418,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -1418,7 +1426,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -1426,7 +1434,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -1434,7 +1442,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -1442,7 +1450,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -1450,7 +1458,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -1458,7 +1466,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -1466,7 +1474,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -1474,7 +1482,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -1482,7 +1490,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -1490,7 +1498,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -1498,7 +1506,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -1506,7 +1514,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -1514,7 +1522,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -1522,7 +1530,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -1530,7 +1538,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -1538,7 +1546,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -1546,7 +1554,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -1554,7 +1562,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -1562,7 +1570,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -1570,7 +1578,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -1578,7 +1586,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -1586,7 +1594,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -1594,7 +1602,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -1602,7 +1610,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -1610,19 +1618,14 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>244</v>
-      </c>
-      <c r="B159">
-        <v>0</v>
-      </c>
+      <c r="A159" s="1"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
@@ -1749,9 +1752,6 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:A158">
@@ -3046,7 +3046,7 @@
   <dimension ref="A1:B158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4325,7 +4325,7 @@
   <dimension ref="A1:B158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C158"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>